<commit_message>
trying to fix some import bugs
</commit_message>
<xml_diff>
--- a/app-server/src/main/resources/2021_organizers.xlsx
+++ b/app-server/src/main/resources/2021_organizers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bushong/code/acmsac/app-server/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0500E08A-4292-9A43-8D98-216F38584729}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93A2F8-2DD9-CA44-B341-1C08BBD6D105}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="15940" xr2:uid="{FE799E17-B61D-1342-B0EB-A182A70A4A23}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>First Name</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>eunjee_song@baylor.edu</t>
+  </si>
+  <si>
+    <t>Vincent</t>
+  </si>
+  <si>
+    <t>Bushong</t>
+  </si>
+  <si>
+    <t>vinbush@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -525,11 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75648735-C5DF-AE4B-ABC1-5FA0B6013742}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,6 +728,23 @@
       </c>
       <c r="E11" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -733,6 +759,7 @@
     <hyperlink ref="C9" r:id="rId8" display="mailto:a.bechini@ing.unipi.it" xr:uid="{583B4799-E1AB-224A-8367-E195B298C22E}"/>
     <hyperlink ref="C10" r:id="rId9" display="mailto:rosa.meo@unito.it" xr:uid="{8FA47EA4-5333-D744-AEDE-7D6C930FE1BE}"/>
     <hyperlink ref="C11" r:id="rId10" display="mailto:jyheo@hansung.ac.kr" xr:uid="{79371164-6B48-BC48-B260-6A5C4CA69C0A}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{BCE0BDBC-3DD8-5A4C-AFE8-3F134320D51B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>